<commit_message>
update inferLayout for fakeScales
</commit_message>
<xml_diff>
--- a/inst/extdata/example2_miss.xlsx
+++ b/inst/extdata/example2_miss.xlsx
@@ -6,14 +6,13 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Students" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Schools" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t xml:space="preserve">Var.name</t>
   </si>
@@ -81,6 +80,27 @@
     <t xml:space="preserve">skala1_item3</t>
   </si>
   <si>
+    <t xml:space="preserve">skala_fake_item1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keinerlei Ahnung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kaum Ahnung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">etwas Ahnung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">viel Ahnung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skala_fake_item2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skala_fake_item3</t>
+  </si>
+  <si>
     <t xml:space="preserve">pvkat_1</t>
   </si>
   <si>
@@ -112,21 +132,6 @@
   </si>
   <si>
     <t xml:space="preserve">pvkat_5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">schooltype</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Omitted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Primary School</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Secondary School</t>
-  </si>
-  <si>
-    <t xml:space="preserve">schoolsize</t>
   </si>
 </sst>
 </file>
@@ -851,51 +856,45 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>1</v>
+        <v>-97</v>
       </c>
       <c r="C24" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" t="s">
-        <v>23</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D24"/>
       <c r="E24" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B25" t="n">
-        <v>2</v>
+        <v>-98</v>
       </c>
       <c r="C25" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" t="s">
-        <v>24</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D25"/>
       <c r="E25" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B26" t="n">
-        <v>3</v>
+        <v>-99</v>
       </c>
       <c r="C26" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" t="s">
-        <v>25</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D26"/>
       <c r="E26" t="s">
         <v>8</v>
       </c>
@@ -905,13 +904,13 @@
         <v>27</v>
       </c>
       <c r="B27" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C27" t="s">
         <v>8</v>
       </c>
       <c r="D27" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E27" t="s">
         <v>8</v>
@@ -922,13 +921,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C28" t="s">
         <v>8</v>
       </c>
       <c r="D28" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E28" t="s">
         <v>8</v>
@@ -936,16 +935,16 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C29" t="s">
         <v>8</v>
       </c>
       <c r="D29" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E29" t="s">
         <v>8</v>
@@ -953,16 +952,16 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B30" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C30" t="s">
         <v>8</v>
       </c>
       <c r="D30" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E30" t="s">
         <v>8</v>
@@ -970,67 +969,61 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B31" t="n">
-        <v>2</v>
+        <v>-97</v>
       </c>
       <c r="C31" t="s">
-        <v>8</v>
-      </c>
-      <c r="D31" t="s">
-        <v>24</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D31"/>
       <c r="E31" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B32" t="n">
-        <v>3</v>
+        <v>-98</v>
       </c>
       <c r="C32" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" t="s">
-        <v>25</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D32"/>
       <c r="E32" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B33" t="n">
-        <v>4</v>
+        <v>-99</v>
       </c>
       <c r="C33" t="s">
-        <v>8</v>
-      </c>
-      <c r="D33" t="s">
-        <v>26</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D33"/>
       <c r="E33" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B34" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C34" t="s">
         <v>8</v>
       </c>
       <c r="D34" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E34" t="s">
         <v>8</v>
@@ -1038,16 +1031,16 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B35" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C35" t="s">
         <v>8</v>
       </c>
       <c r="D35" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E35" t="s">
         <v>8</v>
@@ -1055,16 +1048,16 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B36" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C36" t="s">
         <v>8</v>
       </c>
       <c r="D36" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E36" t="s">
         <v>8</v>
@@ -1072,16 +1065,16 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B37" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C37" t="s">
         <v>8</v>
       </c>
       <c r="D37" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E37" t="s">
         <v>8</v>
@@ -1089,67 +1082,61 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B38" t="n">
-        <v>4</v>
+        <v>-97</v>
       </c>
       <c r="C38" t="s">
-        <v>8</v>
-      </c>
-      <c r="D38" t="s">
-        <v>26</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D38"/>
       <c r="E38" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B39" t="n">
-        <v>5</v>
+        <v>-98</v>
       </c>
       <c r="C39" t="s">
-        <v>8</v>
-      </c>
-      <c r="D39" t="s">
-        <v>28</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D39"/>
       <c r="E39" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B40" t="n">
-        <v>1</v>
+        <v>-99</v>
       </c>
       <c r="C40" t="s">
-        <v>8</v>
-      </c>
-      <c r="D40" t="s">
-        <v>23</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D40"/>
       <c r="E40" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C41" t="s">
         <v>8</v>
       </c>
       <c r="D41" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E41" t="s">
         <v>8</v>
@@ -1157,16 +1144,16 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
+        <v>29</v>
+      </c>
+      <c r="B42" t="n">
+        <v>2</v>
+      </c>
+      <c r="C42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" t="s">
         <v>31</v>
-      </c>
-      <c r="B42" t="n">
-        <v>3</v>
-      </c>
-      <c r="C42" t="s">
-        <v>8</v>
-      </c>
-      <c r="D42" t="s">
-        <v>25</v>
       </c>
       <c r="E42" t="s">
         <v>8</v>
@@ -1174,16 +1161,16 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B43" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C43" t="s">
         <v>8</v>
       </c>
       <c r="D43" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E43" t="s">
         <v>8</v>
@@ -1191,16 +1178,16 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B44" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C44" t="s">
         <v>8</v>
       </c>
       <c r="D44" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="E44" t="s">
         <v>8</v>
@@ -1208,7 +1195,7 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B45" t="n">
         <v>1</v>
@@ -1217,7 +1204,7 @@
         <v>8</v>
       </c>
       <c r="D45" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E45" t="s">
         <v>8</v>
@@ -1225,7 +1212,7 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B46" t="n">
         <v>2</v>
@@ -1234,7 +1221,7 @@
         <v>8</v>
       </c>
       <c r="D46" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="E46" t="s">
         <v>8</v>
@@ -1242,7 +1229,7 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B47" t="n">
         <v>3</v>
@@ -1251,7 +1238,7 @@
         <v>8</v>
       </c>
       <c r="D47" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="E47" t="s">
         <v>8</v>
@@ -1259,7 +1246,7 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B48" t="n">
         <v>4</v>
@@ -1268,7 +1255,7 @@
         <v>8</v>
       </c>
       <c r="D48" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="E48" t="s">
         <v>8</v>
@@ -1276,7 +1263,7 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B49" t="n">
         <v>5</v>
@@ -1285,108 +1272,366 @@
         <v>8</v>
       </c>
       <c r="D49" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="E49" t="s">
         <v>8</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="50">
+      <c r="A50" t="s">
+        <v>29</v>
+      </c>
+      <c r="B50" t="n">
+        <v>5</v>
+      </c>
+      <c r="C50" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50" t="s">
+        <v>35</v>
+      </c>
+      <c r="E50" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>36</v>
+      </c>
+      <c r="B51" t="n">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C51" t="s">
+        <v>8</v>
+      </c>
+      <c r="D51" t="s">
+        <v>30</v>
+      </c>
+      <c r="E51" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>36</v>
+      </c>
+      <c r="B52" t="n">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C52" t="s">
+        <v>8</v>
+      </c>
+      <c r="D52" t="s">
+        <v>31</v>
+      </c>
+      <c r="E52" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>36</v>
+      </c>
+      <c r="B53" t="n">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="C53" t="s">
+        <v>8</v>
+      </c>
+      <c r="D53" t="s">
+        <v>32</v>
+      </c>
+      <c r="E53" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>36</v>
+      </c>
+      <c r="B54" t="n">
         <v>4</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
+      <c r="C54" t="s">
+        <v>8</v>
+      </c>
+      <c r="D54" t="s">
         <v>33</v>
       </c>
-      <c r="B2" t="n">
-        <v>-99</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
+      <c r="E54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>36</v>
+      </c>
+      <c r="B55" t="n">
+        <v>5</v>
+      </c>
+      <c r="C55" t="s">
+        <v>8</v>
+      </c>
+      <c r="D55" t="s">
+        <v>35</v>
+      </c>
+      <c r="E55" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>37</v>
+      </c>
+      <c r="B56" t="n">
+        <v>1</v>
+      </c>
+      <c r="C56" t="s">
+        <v>8</v>
+      </c>
+      <c r="D56" t="s">
+        <v>30</v>
+      </c>
+      <c r="E56" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>37</v>
+      </c>
+      <c r="B57" t="n">
+        <v>2</v>
+      </c>
+      <c r="C57" t="s">
+        <v>8</v>
+      </c>
+      <c r="D57" t="s">
+        <v>31</v>
+      </c>
+      <c r="E57" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>37</v>
+      </c>
+      <c r="B58" t="n">
+        <v>3</v>
+      </c>
+      <c r="C58" t="s">
+        <v>8</v>
+      </c>
+      <c r="D58" t="s">
+        <v>32</v>
+      </c>
+      <c r="E58" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>37</v>
+      </c>
+      <c r="B59" t="n">
+        <v>4</v>
+      </c>
+      <c r="C59" t="s">
+        <v>8</v>
+      </c>
+      <c r="D59" t="s">
         <v>33</v>
       </c>
-      <c r="B3" t="n">
+      <c r="E59" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>37</v>
+      </c>
+      <c r="B60" t="n">
+        <v>5</v>
+      </c>
+      <c r="C60" t="s">
+        <v>8</v>
+      </c>
+      <c r="D60" t="s">
+        <v>35</v>
+      </c>
+      <c r="E60" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>38</v>
+      </c>
+      <c r="B61" t="n">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C61" t="s">
+        <v>8</v>
+      </c>
+      <c r="D61" t="s">
+        <v>30</v>
+      </c>
+      <c r="E61" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>38</v>
+      </c>
+      <c r="B62" t="n">
+        <v>2</v>
+      </c>
+      <c r="C62" t="s">
+        <v>8</v>
+      </c>
+      <c r="D62" t="s">
+        <v>31</v>
+      </c>
+      <c r="E62" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>38</v>
+      </c>
+      <c r="B63" t="n">
+        <v>3</v>
+      </c>
+      <c r="C63" t="s">
+        <v>8</v>
+      </c>
+      <c r="D63" t="s">
+        <v>32</v>
+      </c>
+      <c r="E63" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>38</v>
+      </c>
+      <c r="B64" t="n">
+        <v>4</v>
+      </c>
+      <c r="C64" t="s">
+        <v>8</v>
+      </c>
+      <c r="D64" t="s">
+        <v>33</v>
+      </c>
+      <c r="E64" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>38</v>
+      </c>
+      <c r="B65" t="n">
+        <v>5</v>
+      </c>
+      <c r="C65" t="s">
+        <v>8</v>
+      </c>
+      <c r="D65" t="s">
         <v>35</v>
       </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
+      <c r="E65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>39</v>
+      </c>
+      <c r="B66" t="n">
+        <v>1</v>
+      </c>
+      <c r="C66" t="s">
+        <v>8</v>
+      </c>
+      <c r="D66" t="s">
+        <v>30</v>
+      </c>
+      <c r="E66" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>39</v>
+      </c>
+      <c r="B67" t="n">
+        <v>2</v>
+      </c>
+      <c r="C67" t="s">
+        <v>8</v>
+      </c>
+      <c r="D67" t="s">
+        <v>31</v>
+      </c>
+      <c r="E67" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>39</v>
+      </c>
+      <c r="B68" t="n">
+        <v>3</v>
+      </c>
+      <c r="C68" t="s">
+        <v>8</v>
+      </c>
+      <c r="D68" t="s">
+        <v>32</v>
+      </c>
+      <c r="E68" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>39</v>
+      </c>
+      <c r="B69" t="n">
+        <v>4</v>
+      </c>
+      <c r="C69" t="s">
+        <v>8</v>
+      </c>
+      <c r="D69" t="s">
         <v>33</v>
       </c>
-      <c r="B4" t="n">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" t="n">
-        <v>-99</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="E69" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>39</v>
+      </c>
+      <c r="B70" t="n">
+        <v>5</v>
+      </c>
+      <c r="C70" t="s">
+        <v>8</v>
+      </c>
+      <c r="D70" t="s">
+        <v>35</v>
+      </c>
+      <c r="E70" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>